<commit_message>
Ajuste para poder capturar fechas
</commit_message>
<xml_diff>
--- a/src/pueba.xlsx
+++ b/src/pueba.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\node-excel-to-csv\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\node-xlsx-to-concatenated-txt\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC90496-A7E8-4A8C-9829-49B2334AB81C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E28ECB-658C-493F-B2CD-9C6F057DEF2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0E97C280-4BE1-4674-804A-D0CC908590F2}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Nombre</t>
   </si>
@@ -59,12 +59,21 @@
   </si>
   <si>
     <t>Bicho</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Hora</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -94,8 +103,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,56 +426,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B9D59B-B106-4AA8-9303-9DBBE9221074}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="11.42578125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>24</v>
       </c>
+      <c r="D2" s="2">
+        <v>44732</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.69791666666666663</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>24</v>
       </c>
+      <c r="D3" s="2">
+        <v>44732</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.53125</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>35</v>
+      </c>
+      <c r="D4" s="2">
+        <v>44732</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.40625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agrega codificacion utf8 para caracteres especiales
</commit_message>
<xml_diff>
--- a/src/pueba.xlsx
+++ b/src/pueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\node-xlsx-to-concatenated-txt\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E28ECB-658C-493F-B2CD-9C6F057DEF2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57113F24-161B-4F1D-809C-E14CD3724FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0E97C280-4BE1-4674-804A-D0CC908590F2}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Nombre</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>Hora</t>
+  </si>
+  <si>
+    <t>Nuñez</t>
   </si>
 </sst>
 </file>
@@ -426,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B9D59B-B106-4AA8-9303-9DBBE9221074}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,6 +508,23 @@
         <v>0.40625</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1">
+        <v>21</v>
+      </c>
+      <c r="D5" s="2">
+        <v>44732</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.86458333333333337</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>